<commit_message>
- First work on STA plots (WIP) - Changed output filenames in plots of weights and Smarttester - Summary stats for chert+bamboo for weight data
</commit_message>
<xml_diff>
--- a/analysis/stats/ISEA_use-wear_Weights-stats.xlsx
+++ b/analysis/stats/ISEA_use-wear_Weights-stats.xlsx
@@ -9,6 +9,7 @@
   <sheets>
     <sheet name="Chert type" sheetId="1" r:id="rId1"/>
     <sheet name="Bamboo species" sheetId="2" r:id="rId2"/>
+    <sheet name="Chert+Bamboo" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -812,4 +813,383 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:T5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" s="1" customFormat="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Chert_type</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Bamboo_sp</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Weight_before.n</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Weight_before.min</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Weight_before.max</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Weight_before.mean</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Weight_before.median</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Weight_before.sd</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Weight_after.n</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Weight_after.min</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Weight_after.max</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Weight_after.mean</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Weight_after.median</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>Weight_after.sd</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>Weight_diff.n</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>Weight_diff.min</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>Weight_diff.max</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>Weight_diff.mean</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>Weight_diff.median</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>Weight_diff.sd</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Bambusa blumeana</t>
+        </is>
+      </c>
+      <c r="C2">
+        <v>3</v>
+      </c>
+      <c r="D2">
+        <v>16.69</v>
+      </c>
+      <c r="E2">
+        <v>30.07</v>
+      </c>
+      <c r="F2">
+        <v>25.13666666666667</v>
+      </c>
+      <c r="G2">
+        <v>28.65</v>
+      </c>
+      <c r="H2">
+        <v>7.349403603921431</v>
+      </c>
+      <c r="I2">
+        <v>3</v>
+      </c>
+      <c r="J2">
+        <v>16.66</v>
+      </c>
+      <c r="K2">
+        <v>30</v>
+      </c>
+      <c r="L2">
+        <v>25.09333333333333</v>
+      </c>
+      <c r="M2">
+        <v>28.62</v>
+      </c>
+      <c r="N2">
+        <v>7.336002544528821</v>
+      </c>
+      <c r="O2">
+        <v>3</v>
+      </c>
+      <c r="P2">
+        <v>0.02999999999999758</v>
+      </c>
+      <c r="Q2">
+        <v>0.07000000000000028</v>
+      </c>
+      <c r="R2">
+        <v>0.043333333333333</v>
+      </c>
+      <c r="S2">
+        <v>0.03000000000000114</v>
+      </c>
+      <c r="T2">
+        <v>0.02309401076758556</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Schizostachum lima</t>
+        </is>
+      </c>
+      <c r="C3">
+        <v>3</v>
+      </c>
+      <c r="D3">
+        <v>15.32</v>
+      </c>
+      <c r="E3">
+        <v>24.6</v>
+      </c>
+      <c r="F3">
+        <v>19.39</v>
+      </c>
+      <c r="G3">
+        <v>18.25</v>
+      </c>
+      <c r="H3">
+        <v>4.743869728396851</v>
+      </c>
+      <c r="I3">
+        <v>3</v>
+      </c>
+      <c r="J3">
+        <v>15.31</v>
+      </c>
+      <c r="K3">
+        <v>24.44</v>
+      </c>
+      <c r="L3">
+        <v>19.33</v>
+      </c>
+      <c r="M3">
+        <v>18.24</v>
+      </c>
+      <c r="N3">
+        <v>4.661576986385617</v>
+      </c>
+      <c r="O3">
+        <v>3</v>
+      </c>
+      <c r="P3">
+        <v>0.009999999999999787</v>
+      </c>
+      <c r="Q3">
+        <v>0.1600000000000001</v>
+      </c>
+      <c r="R3">
+        <v>0.0600000000000005</v>
+      </c>
+      <c r="S3">
+        <v>0.01000000000000156</v>
+      </c>
+      <c r="T3">
+        <v>0.08660254037844356</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Bambusa blumeana</t>
+        </is>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="D4">
+        <v>10.25</v>
+      </c>
+      <c r="E4">
+        <v>21.52</v>
+      </c>
+      <c r="F4">
+        <v>16.15333333333333</v>
+      </c>
+      <c r="G4">
+        <v>16.69</v>
+      </c>
+      <c r="H4">
+        <v>5.654134180697636</v>
+      </c>
+      <c r="I4">
+        <v>3</v>
+      </c>
+      <c r="J4">
+        <v>10.04</v>
+      </c>
+      <c r="K4">
+        <v>21.5</v>
+      </c>
+      <c r="L4">
+        <v>16.07</v>
+      </c>
+      <c r="M4">
+        <v>16.67</v>
+      </c>
+      <c r="N4">
+        <v>5.753511970961736</v>
+      </c>
+      <c r="O4">
+        <v>3</v>
+      </c>
+      <c r="P4">
+        <v>0.01999999999999957</v>
+      </c>
+      <c r="Q4">
+        <v>0.2100000000000009</v>
+      </c>
+      <c r="R4">
+        <v>0.08333333333333333</v>
+      </c>
+      <c r="S4">
+        <v>0.01999999999999957</v>
+      </c>
+      <c r="T4">
+        <v>0.1096965511460296</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Schizostachum lima</t>
+        </is>
+      </c>
+      <c r="C5">
+        <v>3</v>
+      </c>
+      <c r="D5">
+        <v>13.49</v>
+      </c>
+      <c r="E5">
+        <v>17.04</v>
+      </c>
+      <c r="F5">
+        <v>15.76333333333333</v>
+      </c>
+      <c r="G5">
+        <v>16.76</v>
+      </c>
+      <c r="H5">
+        <v>1.973735882364541</v>
+      </c>
+      <c r="I5">
+        <v>3</v>
+      </c>
+      <c r="J5">
+        <v>13.48</v>
+      </c>
+      <c r="K5">
+        <v>17</v>
+      </c>
+      <c r="L5">
+        <v>15.74</v>
+      </c>
+      <c r="M5">
+        <v>16.74</v>
+      </c>
+      <c r="N5">
+        <v>1.96153001506477</v>
+      </c>
+      <c r="O5">
+        <v>3</v>
+      </c>
+      <c r="P5">
+        <v>0.009999999999999787</v>
+      </c>
+      <c r="Q5">
+        <v>0.03999999999999915</v>
+      </c>
+      <c r="R5">
+        <v>0.02333333333333402</v>
+      </c>
+      <c r="S5">
+        <v>0.02000000000000313</v>
+      </c>
+      <c r="T5">
+        <v>0.01527525231651875</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>